<commit_message>
updates to template.xlsx, create theme.js, and formatting updates (font family changed to Yu Gothic)
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="77" documentId="8_{555B2289-9F82-4653-BCD0-D67F31357259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CE41AC-585E-48A0-9802-CE8E50390320}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operation Standards" sheetId="6" r:id="rId1"/>
@@ -5262,41 +5262,454 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5335,454 +5748,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5820,6 +5820,63 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="justify"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5876,63 +5933,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -11772,8 +11772,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B3:AD122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115:Z122"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.75"/>
@@ -12310,7 +12310,7 @@
   </sheetPr>
   <dimension ref="A1:BM106"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="AZ20" sqref="AZ20"/>
     </sheetView>
   </sheetViews>
@@ -12345,9 +12345,9 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="520"/>
-      <c r="C1" s="521"/>
-      <c r="D1" s="521"/>
+      <c r="B1" s="570"/>
+      <c r="C1" s="571"/>
+      <c r="D1" s="571"/>
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -12412,17 +12412,17 @@
       </c>
     </row>
     <row r="3" spans="1:52" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="530" t="s">
+      <c r="A3" s="580" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="531"/>
-      <c r="C3" s="512" t="s">
+      <c r="B3" s="581"/>
+      <c r="C3" s="564" t="s">
         <v>211</v>
       </c>
-      <c r="D3" s="513"/>
-      <c r="E3" s="513"/>
-      <c r="F3" s="513"/>
-      <c r="G3" s="514"/>
+      <c r="D3" s="565"/>
+      <c r="E3" s="565"/>
+      <c r="F3" s="565"/>
+      <c r="G3" s="566"/>
       <c r="H3" s="227" t="s">
         <v>4</v>
       </c>
@@ -12457,13 +12457,13 @@
       <c r="AZ3" s="311"/>
     </row>
     <row r="4" spans="1:52" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="532"/>
-      <c r="B4" s="533"/>
-      <c r="C4" s="515"/>
-      <c r="D4" s="515"/>
-      <c r="E4" s="515"/>
-      <c r="F4" s="515"/>
-      <c r="G4" s="516"/>
+      <c r="A4" s="582"/>
+      <c r="B4" s="583"/>
+      <c r="C4" s="538"/>
+      <c r="D4" s="538"/>
+      <c r="E4" s="538"/>
+      <c r="F4" s="538"/>
+      <c r="G4" s="567"/>
       <c r="H4" s="31"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32" t="s">
@@ -12473,10 +12473,10 @@
       <c r="L4" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="561"/>
-      <c r="N4" s="562"/>
-      <c r="O4" s="562"/>
-      <c r="P4" s="563"/>
+      <c r="M4" s="548"/>
+      <c r="N4" s="549"/>
+      <c r="O4" s="549"/>
+      <c r="P4" s="550"/>
       <c r="Q4" s="195" t="s">
         <v>8</v>
       </c>
@@ -12500,85 +12500,85 @@
       <c r="AZ4" s="311"/>
     </row>
     <row r="5" spans="1:52" ht="12" customHeight="1">
-      <c r="A5" s="534" t="s">
+      <c r="A5" s="584" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="535"/>
-      <c r="C5" s="517" t="s">
+      <c r="B5" s="585"/>
+      <c r="C5" s="568" t="s">
         <v>211</v>
       </c>
-      <c r="D5" s="518"/>
-      <c r="E5" s="518"/>
-      <c r="F5" s="518"/>
-      <c r="G5" s="519"/>
+      <c r="D5" s="484"/>
+      <c r="E5" s="484"/>
+      <c r="F5" s="484"/>
+      <c r="G5" s="569"/>
       <c r="H5" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="541"/>
-      <c r="J5" s="541"/>
-      <c r="K5" s="541"/>
-      <c r="L5" s="542"/>
-      <c r="M5" s="564"/>
-      <c r="N5" s="565"/>
-      <c r="O5" s="565"/>
-      <c r="P5" s="566"/>
+      <c r="I5" s="530"/>
+      <c r="J5" s="530"/>
+      <c r="K5" s="530"/>
+      <c r="L5" s="531"/>
+      <c r="M5" s="551"/>
+      <c r="N5" s="552"/>
+      <c r="O5" s="552"/>
+      <c r="P5" s="553"/>
       <c r="Q5" s="196"/>
-      <c r="R5" s="553"/>
-      <c r="S5" s="554"/>
-      <c r="T5" s="553"/>
-      <c r="U5" s="559"/>
+      <c r="R5" s="542"/>
+      <c r="S5" s="543"/>
+      <c r="T5" s="542"/>
+      <c r="U5" s="476"/>
       <c r="V5" s="97"/>
-      <c r="W5" s="573" t="s">
+      <c r="W5" s="560" t="s">
         <v>121</v>
       </c>
-      <c r="X5" s="574"/>
-      <c r="Y5" s="573" t="s">
+      <c r="X5" s="561"/>
+      <c r="Y5" s="560" t="s">
         <v>122</v>
       </c>
-      <c r="Z5" s="574"/>
-      <c r="AA5" s="570" t="s">
+      <c r="Z5" s="561"/>
+      <c r="AA5" s="557" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="571"/>
-      <c r="AC5" s="572"/>
+      <c r="AB5" s="558"/>
+      <c r="AC5" s="559"/>
       <c r="AY5" t="s">
         <v>105</v>
       </c>
       <c r="AZ5" s="311"/>
     </row>
     <row r="6" spans="1:52" ht="12.6" customHeight="1">
-      <c r="A6" s="532"/>
-      <c r="B6" s="533"/>
-      <c r="C6" s="515"/>
-      <c r="D6" s="515"/>
-      <c r="E6" s="515"/>
-      <c r="F6" s="515"/>
-      <c r="G6" s="516"/>
+      <c r="A6" s="582"/>
+      <c r="B6" s="583"/>
+      <c r="C6" s="538"/>
+      <c r="D6" s="538"/>
+      <c r="E6" s="538"/>
+      <c r="F6" s="538"/>
+      <c r="G6" s="567"/>
       <c r="H6" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="541"/>
-      <c r="J6" s="541"/>
-      <c r="K6" s="541"/>
-      <c r="L6" s="542"/>
-      <c r="M6" s="564"/>
-      <c r="N6" s="565"/>
-      <c r="O6" s="565"/>
-      <c r="P6" s="566"/>
+      <c r="I6" s="530"/>
+      <c r="J6" s="530"/>
+      <c r="K6" s="530"/>
+      <c r="L6" s="531"/>
+      <c r="M6" s="551"/>
+      <c r="N6" s="552"/>
+      <c r="O6" s="552"/>
+      <c r="P6" s="553"/>
       <c r="Q6" s="197" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="555"/>
-      <c r="S6" s="556"/>
-      <c r="T6" s="555"/>
-      <c r="U6" s="497"/>
-      <c r="V6" s="575" t="s">
+      <c r="R6" s="544"/>
+      <c r="S6" s="545"/>
+      <c r="T6" s="544"/>
+      <c r="U6" s="477"/>
+      <c r="V6" s="562" t="s">
         <v>12</v>
       </c>
-      <c r="W6" s="543"/>
-      <c r="X6" s="544"/>
-      <c r="Y6" s="547"/>
-      <c r="Z6" s="518"/>
+      <c r="W6" s="532"/>
+      <c r="X6" s="533"/>
+      <c r="Y6" s="536"/>
+      <c r="Z6" s="484"/>
       <c r="AA6" s="173"/>
       <c r="AC6" s="98"/>
       <c r="AY6" t="s">
@@ -12587,36 +12587,36 @@
       <c r="AZ6" s="311"/>
     </row>
     <row r="7" spans="1:52" ht="12" customHeight="1">
-      <c r="A7" s="534" t="s">
+      <c r="A7" s="584" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="535"/>
-      <c r="C7" s="517"/>
-      <c r="D7" s="518"/>
-      <c r="E7" s="518"/>
-      <c r="F7" s="518"/>
-      <c r="G7" s="519"/>
+      <c r="B7" s="585"/>
+      <c r="C7" s="568"/>
+      <c r="D7" s="484"/>
+      <c r="E7" s="484"/>
+      <c r="F7" s="484"/>
+      <c r="G7" s="569"/>
       <c r="H7" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="539"/>
-      <c r="J7" s="539"/>
-      <c r="K7" s="539"/>
-      <c r="L7" s="540"/>
-      <c r="M7" s="564"/>
-      <c r="N7" s="565"/>
-      <c r="O7" s="565"/>
-      <c r="P7" s="566"/>
+      <c r="I7" s="526"/>
+      <c r="J7" s="526"/>
+      <c r="K7" s="526"/>
+      <c r="L7" s="527"/>
+      <c r="M7" s="551"/>
+      <c r="N7" s="552"/>
+      <c r="O7" s="552"/>
+      <c r="P7" s="553"/>
       <c r="Q7" s="198"/>
-      <c r="R7" s="557"/>
-      <c r="S7" s="558"/>
-      <c r="T7" s="557"/>
-      <c r="U7" s="560"/>
-      <c r="V7" s="576"/>
-      <c r="W7" s="545"/>
-      <c r="X7" s="546"/>
-      <c r="Y7" s="548"/>
-      <c r="Z7" s="515"/>
+      <c r="R7" s="546"/>
+      <c r="S7" s="547"/>
+      <c r="T7" s="546"/>
+      <c r="U7" s="475"/>
+      <c r="V7" s="563"/>
+      <c r="W7" s="534"/>
+      <c r="X7" s="535"/>
+      <c r="Y7" s="537"/>
+      <c r="Z7" s="538"/>
       <c r="AA7" s="125" t="s">
         <v>13</v>
       </c>
@@ -12630,36 +12630,36 @@
       <c r="AZ7" s="311"/>
     </row>
     <row r="8" spans="1:52" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A8" s="532"/>
-      <c r="B8" s="533"/>
-      <c r="C8" s="515"/>
-      <c r="D8" s="515"/>
-      <c r="E8" s="515"/>
-      <c r="F8" s="515"/>
-      <c r="G8" s="516"/>
+      <c r="A8" s="582"/>
+      <c r="B8" s="583"/>
+      <c r="C8" s="538"/>
+      <c r="D8" s="538"/>
+      <c r="E8" s="538"/>
+      <c r="F8" s="538"/>
+      <c r="G8" s="567"/>
       <c r="H8" s="27"/>
-      <c r="I8" s="505"/>
-      <c r="J8" s="505"/>
-      <c r="K8" s="505"/>
-      <c r="L8" s="506"/>
-      <c r="M8" s="567"/>
-      <c r="N8" s="568"/>
-      <c r="O8" s="568"/>
-      <c r="P8" s="569"/>
+      <c r="I8" s="528"/>
+      <c r="J8" s="528"/>
+      <c r="K8" s="528"/>
+      <c r="L8" s="529"/>
+      <c r="M8" s="554"/>
+      <c r="N8" s="555"/>
+      <c r="O8" s="555"/>
+      <c r="P8" s="556"/>
       <c r="Q8" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="551"/>
-      <c r="S8" s="617"/>
-      <c r="T8" s="551"/>
-      <c r="U8" s="618"/>
+      <c r="R8" s="466"/>
+      <c r="S8" s="467"/>
+      <c r="T8" s="466"/>
+      <c r="U8" s="468"/>
       <c r="V8" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="W8" s="549"/>
-      <c r="X8" s="550"/>
-      <c r="Y8" s="551"/>
-      <c r="Z8" s="552"/>
+      <c r="W8" s="539"/>
+      <c r="X8" s="540"/>
+      <c r="Y8" s="466"/>
+      <c r="Z8" s="541"/>
       <c r="AA8" s="126" t="str">
         <f>IF(AND(AB14=0,AB15&lt;&gt;0),"X","")</f>
         <v/>
@@ -12680,10 +12680,10 @@
       </c>
       <c r="B9" s="27"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="493" t="s">
+      <c r="H9" s="588" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="500"/>
+      <c r="I9" s="592"/>
       <c r="J9" s="189" t="s">
         <v>99</v>
       </c>
@@ -12693,25 +12693,25 @@
       <c r="N9" s="189"/>
       <c r="O9" s="189"/>
       <c r="P9" s="190"/>
-      <c r="Q9" s="619" t="s">
+      <c r="Q9" s="469" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="620"/>
-      <c r="S9" s="623"/>
-      <c r="T9" s="624"/>
-      <c r="U9" s="624"/>
-      <c r="V9" s="470" t="s">
+      <c r="R9" s="470"/>
+      <c r="S9" s="473"/>
+      <c r="T9" s="474"/>
+      <c r="U9" s="474"/>
+      <c r="V9" s="617" t="s">
         <v>159</v>
       </c>
-      <c r="W9" s="471"/>
-      <c r="X9" s="471"/>
-      <c r="Y9" s="471"/>
-      <c r="Z9" s="471"/>
-      <c r="AA9" s="472"/>
-      <c r="AB9" s="468" t="s">
+      <c r="W9" s="618"/>
+      <c r="X9" s="618"/>
+      <c r="Y9" s="618"/>
+      <c r="Z9" s="618"/>
+      <c r="AA9" s="619"/>
+      <c r="AB9" s="615" t="s">
         <v>158</v>
       </c>
-      <c r="AC9" s="466" t="s">
+      <c r="AC9" s="613" t="s">
         <v>157</v>
       </c>
       <c r="AY9" t="s">
@@ -12726,13 +12726,13 @@
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
-      <c r="E10" s="496" t="s">
+      <c r="E10" s="591" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="496"/>
-      <c r="G10" s="497"/>
-      <c r="H10" s="494"/>
-      <c r="I10" s="501"/>
+      <c r="F10" s="591"/>
+      <c r="G10" s="477"/>
+      <c r="H10" s="589"/>
+      <c r="I10" s="593"/>
       <c r="J10" s="191"/>
       <c r="K10" s="191"/>
       <c r="L10" s="191"/>
@@ -12740,19 +12740,19 @@
       <c r="N10" s="191"/>
       <c r="O10" s="191"/>
       <c r="P10" s="192"/>
-      <c r="Q10" s="621"/>
-      <c r="R10" s="622"/>
-      <c r="S10" s="560"/>
-      <c r="T10" s="560"/>
-      <c r="U10" s="560"/>
-      <c r="V10" s="473"/>
-      <c r="W10" s="474"/>
-      <c r="X10" s="474"/>
-      <c r="Y10" s="474"/>
-      <c r="Z10" s="474"/>
-      <c r="AA10" s="475"/>
-      <c r="AB10" s="469"/>
-      <c r="AC10" s="467"/>
+      <c r="Q10" s="471"/>
+      <c r="R10" s="472"/>
+      <c r="S10" s="475"/>
+      <c r="T10" s="475"/>
+      <c r="U10" s="475"/>
+      <c r="V10" s="620"/>
+      <c r="W10" s="621"/>
+      <c r="X10" s="621"/>
+      <c r="Y10" s="621"/>
+      <c r="Z10" s="621"/>
+      <c r="AA10" s="622"/>
+      <c r="AB10" s="616"/>
+      <c r="AC10" s="614"/>
       <c r="AY10" s="95" t="s">
         <v>111</v>
       </c>
@@ -12765,13 +12765,13 @@
       </c>
       <c r="C11" s="462"/>
       <c r="D11"/>
-      <c r="E11" s="510" t="s">
+      <c r="E11" s="600" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="510"/>
-      <c r="G11" s="511"/>
-      <c r="H11" s="494"/>
-      <c r="I11" s="501"/>
+      <c r="F11" s="600"/>
+      <c r="G11" s="601"/>
+      <c r="H11" s="589"/>
+      <c r="I11" s="593"/>
       <c r="J11" s="191"/>
       <c r="K11" s="191"/>
       <c r="L11" s="191"/>
@@ -12779,23 +12779,23 @@
       <c r="N11" s="191"/>
       <c r="O11" s="191"/>
       <c r="P11" s="192"/>
-      <c r="Q11" s="607" t="s">
+      <c r="Q11" s="483" t="s">
         <v>65</v>
       </c>
-      <c r="R11" s="518"/>
-      <c r="S11" s="559"/>
-      <c r="T11" s="559"/>
-      <c r="U11" s="559"/>
+      <c r="R11" s="484"/>
+      <c r="S11" s="476"/>
+      <c r="T11" s="476"/>
+      <c r="U11" s="476"/>
       <c r="V11" s="203" t="s">
         <v>146</v>
       </c>
       <c r="W11" s="73"/>
-      <c r="X11" s="476" t="s">
+      <c r="X11" s="623" t="s">
         <v>21</v>
       </c>
-      <c r="Y11" s="476"/>
-      <c r="Z11" s="476"/>
-      <c r="AA11" s="477"/>
+      <c r="Y11" s="623"/>
+      <c r="Z11" s="623"/>
+      <c r="AA11" s="624"/>
       <c r="AB11" s="243">
         <f>COUNTIF('IDS Page 1'!$AN$27:$AW$97,"OK")+IFERROR(COUNTIF('IDS Additional Data Sheet'!$AP$6:$AY$47,"OK"),0)</f>
         <v>0</v>
@@ -12817,8 +12817,8 @@
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="495"/>
-      <c r="I12" s="502"/>
+      <c r="H12" s="590"/>
+      <c r="I12" s="594"/>
       <c r="J12" s="193"/>
       <c r="K12" s="193"/>
       <c r="L12" s="193"/>
@@ -12826,21 +12826,21 @@
       <c r="N12" s="193"/>
       <c r="O12" s="193"/>
       <c r="P12" s="194"/>
-      <c r="Q12" s="608"/>
-      <c r="R12" s="608"/>
-      <c r="S12" s="497"/>
-      <c r="T12" s="497"/>
-      <c r="U12" s="497"/>
+      <c r="Q12" s="485"/>
+      <c r="R12" s="485"/>
+      <c r="S12" s="477"/>
+      <c r="T12" s="477"/>
+      <c r="U12" s="477"/>
       <c r="V12" s="203" t="s">
         <v>207</v>
       </c>
       <c r="W12" s="73"/>
-      <c r="X12" s="476" t="s">
+      <c r="X12" s="623" t="s">
         <v>208</v>
       </c>
-      <c r="Y12" s="476"/>
-      <c r="Z12" s="476"/>
-      <c r="AA12" s="477"/>
+      <c r="Y12" s="623"/>
+      <c r="Z12" s="623"/>
+      <c r="AA12" s="624"/>
       <c r="AB12" s="243">
         <f>COUNTIF('IDS Page 1'!$AN$27:$AW$97,"NG")+IFERROR(COUNTIF('IDS Additional Data Sheet'!$AP$6:$AY$47,"NG"),0)</f>
         <v>0</v>
@@ -12857,41 +12857,41 @@
       <c r="AZ12" s="311"/>
     </row>
     <row r="13" spans="1:52" ht="12" customHeight="1" thickBot="1">
-      <c r="A13" s="503" t="s">
+      <c r="A13" s="595" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="504"/>
-      <c r="C13" s="504"/>
-      <c r="D13" s="504"/>
-      <c r="E13" s="504"/>
-      <c r="F13" s="504"/>
-      <c r="G13" s="504"/>
-      <c r="H13" s="505"/>
-      <c r="I13" s="505"/>
-      <c r="J13" s="505"/>
-      <c r="K13" s="505"/>
-      <c r="L13" s="505"/>
-      <c r="M13" s="505"/>
-      <c r="N13" s="505"/>
-      <c r="O13" s="505"/>
-      <c r="P13" s="506"/>
-      <c r="Q13" s="609" t="s">
+      <c r="B13" s="596"/>
+      <c r="C13" s="596"/>
+      <c r="D13" s="596"/>
+      <c r="E13" s="596"/>
+      <c r="F13" s="596"/>
+      <c r="G13" s="596"/>
+      <c r="H13" s="528"/>
+      <c r="I13" s="528"/>
+      <c r="J13" s="528"/>
+      <c r="K13" s="528"/>
+      <c r="L13" s="528"/>
+      <c r="M13" s="528"/>
+      <c r="N13" s="528"/>
+      <c r="O13" s="528"/>
+      <c r="P13" s="529"/>
+      <c r="Q13" s="486" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="610"/>
-      <c r="S13" s="613"/>
-      <c r="T13" s="614"/>
-      <c r="U13" s="614"/>
+      <c r="R13" s="487"/>
+      <c r="S13" s="490"/>
+      <c r="T13" s="491"/>
+      <c r="U13" s="491"/>
       <c r="V13" s="79" t="s">
         <v>60</v>
       </c>
       <c r="W13" s="73"/>
-      <c r="X13" s="485" t="s">
+      <c r="X13" s="609" t="s">
         <v>21</v>
       </c>
-      <c r="Y13" s="485"/>
-      <c r="Z13" s="485"/>
-      <c r="AA13" s="486"/>
+      <c r="Y13" s="609"/>
+      <c r="Z13" s="609"/>
+      <c r="AA13" s="610"/>
       <c r="AB13" s="243">
         <f>COUNTIF('IDS Page 1'!$AD$27:$AM$97,"OK")+IFERROR(COUNTIF('IDS Additional Data Sheet'!$AE$6:$AN$47,"OK"),0)</f>
         <v>0</v>
@@ -12938,23 +12938,23 @@
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-      <c r="Q14" s="611" t="s">
+      <c r="Q14" s="488" t="s">
         <v>110</v>
       </c>
-      <c r="R14" s="612"/>
-      <c r="S14" s="615"/>
-      <c r="T14" s="616"/>
-      <c r="U14" s="616"/>
+      <c r="R14" s="489"/>
+      <c r="S14" s="492"/>
+      <c r="T14" s="493"/>
+      <c r="U14" s="493"/>
       <c r="V14" s="285" t="s">
         <v>61</v>
       </c>
       <c r="W14" s="264"/>
-      <c r="X14" s="487" t="s">
+      <c r="X14" s="611" t="s">
         <v>24</v>
       </c>
-      <c r="Y14" s="487"/>
-      <c r="Z14" s="487"/>
-      <c r="AA14" s="488"/>
+      <c r="Y14" s="611"/>
+      <c r="Z14" s="611"/>
+      <c r="AA14" s="612"/>
       <c r="AB14" s="286">
         <f>COUNTIF('IDS Page 1'!$AD$27:$AM$97,"NG")+IFERROR(COUNTIF('IDS Additional Data Sheet'!$AE$6:$AN$47,"NG"),0)</f>
         <v>0</v>
@@ -12968,20 +12968,20 @@
     <row r="15" spans="1:52" ht="12" customHeight="1">
       <c r="A15" s="122"/>
       <c r="B15" s="39"/>
-      <c r="C15" s="491"/>
-      <c r="D15" s="492"/>
-      <c r="E15" s="491"/>
-      <c r="F15" s="498"/>
-      <c r="G15" s="499"/>
-      <c r="H15" s="499"/>
-      <c r="I15" s="499"/>
-      <c r="J15" s="492"/>
+      <c r="C15" s="500"/>
+      <c r="D15" s="576"/>
+      <c r="E15" s="500"/>
+      <c r="F15" s="574"/>
+      <c r="G15" s="575"/>
+      <c r="H15" s="575"/>
+      <c r="I15" s="575"/>
+      <c r="J15" s="576"/>
       <c r="K15" s="69"/>
       <c r="L15" s="102"/>
       <c r="M15" s="103"/>
-      <c r="N15" s="507"/>
-      <c r="O15" s="508"/>
-      <c r="P15" s="509"/>
+      <c r="N15" s="597"/>
+      <c r="O15" s="598"/>
+      <c r="P15" s="599"/>
       <c r="Q15" s="7" t="s">
         <v>28</v>
       </c>
@@ -12992,19 +12992,19 @@
         <v>30</v>
       </c>
       <c r="U15" s="36"/>
-      <c r="V15" s="482" t="s">
+      <c r="V15" s="606" t="s">
         <v>210</v>
       </c>
-      <c r="W15" s="483"/>
-      <c r="X15" s="483"/>
-      <c r="Y15" s="483"/>
-      <c r="Z15" s="483"/>
-      <c r="AA15" s="484"/>
-      <c r="AB15" s="478">
+      <c r="W15" s="607"/>
+      <c r="X15" s="607"/>
+      <c r="Y15" s="607"/>
+      <c r="Z15" s="607"/>
+      <c r="AA15" s="608"/>
+      <c r="AB15" s="602">
         <f>SUM(AB13:AB14)</f>
         <v>0</v>
       </c>
-      <c r="AC15" s="480" t="str">
+      <c r="AC15" s="604" t="str">
         <f>IF($AB$15=0,"",(AB15/$AB$15)*100)</f>
         <v/>
       </c>
@@ -13013,29 +13013,29 @@
     <row r="16" spans="1:52" ht="12" customHeight="1" thickBot="1">
       <c r="A16" s="122"/>
       <c r="B16" s="39"/>
-      <c r="C16" s="491"/>
-      <c r="D16" s="492"/>
-      <c r="E16" s="491"/>
-      <c r="F16" s="498"/>
-      <c r="G16" s="499"/>
-      <c r="H16" s="499"/>
-      <c r="I16" s="499"/>
-      <c r="J16" s="492"/>
+      <c r="C16" s="500"/>
+      <c r="D16" s="576"/>
+      <c r="E16" s="500"/>
+      <c r="F16" s="574"/>
+      <c r="G16" s="575"/>
+      <c r="H16" s="575"/>
+      <c r="I16" s="575"/>
+      <c r="J16" s="576"/>
       <c r="K16" s="69"/>
       <c r="L16" s="102"/>
       <c r="M16" s="103"/>
-      <c r="N16" s="527"/>
-      <c r="O16" s="528"/>
-      <c r="P16" s="529"/>
+      <c r="N16" s="498"/>
+      <c r="O16" s="499"/>
+      <c r="P16" s="513"/>
       <c r="S16" s="6"/>
-      <c r="V16" s="482"/>
-      <c r="W16" s="483"/>
-      <c r="X16" s="483"/>
-      <c r="Y16" s="483"/>
-      <c r="Z16" s="483"/>
-      <c r="AA16" s="483"/>
-      <c r="AB16" s="479"/>
-      <c r="AC16" s="481"/>
+      <c r="V16" s="606"/>
+      <c r="W16" s="607"/>
+      <c r="X16" s="607"/>
+      <c r="Y16" s="607"/>
+      <c r="Z16" s="607"/>
+      <c r="AA16" s="607"/>
+      <c r="AB16" s="603"/>
+      <c r="AC16" s="605"/>
       <c r="AZ16" s="311"/>
     </row>
     <row r="17" spans="1:65" ht="12" customHeight="1" thickBot="1">
@@ -13052,26 +13052,26 @@
       <c r="K17" s="69"/>
       <c r="L17" s="102"/>
       <c r="M17" s="103"/>
-      <c r="N17" s="527"/>
-      <c r="O17" s="528"/>
-      <c r="P17" s="529"/>
-      <c r="Q17" s="605" t="s">
+      <c r="N17" s="498"/>
+      <c r="O17" s="499"/>
+      <c r="P17" s="513"/>
+      <c r="Q17" s="478" t="s">
         <v>56</v>
       </c>
-      <c r="R17" s="606"/>
-      <c r="S17" s="536"/>
-      <c r="T17" s="537"/>
-      <c r="U17" s="538"/>
+      <c r="R17" s="479"/>
+      <c r="S17" s="480"/>
+      <c r="T17" s="481"/>
+      <c r="U17" s="482"/>
       <c r="V17" s="265" t="s">
         <v>54</v>
       </c>
       <c r="W17" s="200"/>
-      <c r="X17" s="536"/>
-      <c r="Y17" s="537"/>
-      <c r="Z17" s="537"/>
-      <c r="AA17" s="537"/>
-      <c r="AB17" s="537"/>
-      <c r="AC17" s="538"/>
+      <c r="X17" s="480"/>
+      <c r="Y17" s="481"/>
+      <c r="Z17" s="481"/>
+      <c r="AA17" s="481"/>
+      <c r="AB17" s="481"/>
+      <c r="AC17" s="482"/>
       <c r="AZ17" s="311"/>
     </row>
     <row r="18" spans="1:65" ht="12" customHeight="1" thickBot="1">
@@ -13088,28 +13088,28 @@
       <c r="K18" s="69"/>
       <c r="L18" s="102"/>
       <c r="M18" s="103"/>
-      <c r="N18" s="527"/>
-      <c r="O18" s="528"/>
-      <c r="P18" s="529"/>
-      <c r="Q18" s="577" t="s">
+      <c r="N18" s="498"/>
+      <c r="O18" s="499"/>
+      <c r="P18" s="513"/>
+      <c r="Q18" s="494" t="s">
         <v>147</v>
       </c>
-      <c r="R18" s="578"/>
-      <c r="S18" s="587"/>
-      <c r="T18" s="588"/>
-      <c r="U18" s="589"/>
-      <c r="V18" s="581" t="s">
+      <c r="R18" s="495"/>
+      <c r="S18" s="507"/>
+      <c r="T18" s="508"/>
+      <c r="U18" s="509"/>
+      <c r="V18" s="501" t="s">
         <v>55</v>
       </c>
-      <c r="W18" s="582"/>
-      <c r="X18" s="583"/>
-      <c r="Y18" s="584"/>
+      <c r="W18" s="502"/>
+      <c r="X18" s="503"/>
+      <c r="Y18" s="504"/>
       <c r="Z18" s="201" t="s">
         <v>57</v>
       </c>
-      <c r="AA18" s="599"/>
-      <c r="AB18" s="600"/>
-      <c r="AC18" s="601"/>
+      <c r="AA18" s="520"/>
+      <c r="AB18" s="521"/>
+      <c r="AC18" s="522"/>
       <c r="AZ18" s="311"/>
     </row>
     <row r="19" spans="1:65" ht="12" customHeight="1" thickBot="1">
@@ -13126,26 +13126,26 @@
       <c r="K19" s="69"/>
       <c r="L19" s="102"/>
       <c r="M19" s="103"/>
-      <c r="N19" s="527"/>
-      <c r="O19" s="528"/>
-      <c r="P19" s="529"/>
-      <c r="Q19" s="579"/>
-      <c r="R19" s="580"/>
-      <c r="S19" s="590"/>
-      <c r="T19" s="591"/>
-      <c r="U19" s="592"/>
-      <c r="V19" s="581" t="s">
+      <c r="N19" s="498"/>
+      <c r="O19" s="499"/>
+      <c r="P19" s="513"/>
+      <c r="Q19" s="496"/>
+      <c r="R19" s="497"/>
+      <c r="S19" s="510"/>
+      <c r="T19" s="511"/>
+      <c r="U19" s="512"/>
+      <c r="V19" s="501" t="s">
         <v>58</v>
       </c>
-      <c r="W19" s="582"/>
-      <c r="X19" s="536"/>
-      <c r="Y19" s="538"/>
+      <c r="W19" s="502"/>
+      <c r="X19" s="480"/>
+      <c r="Y19" s="482"/>
       <c r="Z19" s="202" t="s">
         <v>66</v>
       </c>
-      <c r="AA19" s="602"/>
-      <c r="AB19" s="603"/>
-      <c r="AC19" s="604"/>
+      <c r="AA19" s="523"/>
+      <c r="AB19" s="524"/>
+      <c r="AC19" s="525"/>
       <c r="AZ19" s="311"/>
     </row>
     <row r="20" spans="1:65" ht="12" customHeight="1" thickBot="1">
@@ -13162,43 +13162,43 @@
       <c r="K20" s="69"/>
       <c r="L20" s="102"/>
       <c r="M20" s="103"/>
-      <c r="N20" s="527"/>
-      <c r="O20" s="528"/>
-      <c r="P20" s="529"/>
-      <c r="Q20" s="585" t="s">
+      <c r="N20" s="498"/>
+      <c r="O20" s="499"/>
+      <c r="P20" s="513"/>
+      <c r="Q20" s="505" t="s">
         <v>67</v>
       </c>
-      <c r="R20" s="586"/>
-      <c r="S20" s="536"/>
-      <c r="T20" s="537"/>
-      <c r="U20" s="537"/>
-      <c r="V20" s="537"/>
-      <c r="W20" s="537"/>
-      <c r="X20" s="537"/>
-      <c r="Y20" s="537"/>
-      <c r="Z20" s="537"/>
-      <c r="AA20" s="537"/>
-      <c r="AB20" s="537"/>
-      <c r="AC20" s="538"/>
+      <c r="R20" s="506"/>
+      <c r="S20" s="480"/>
+      <c r="T20" s="481"/>
+      <c r="U20" s="481"/>
+      <c r="V20" s="481"/>
+      <c r="W20" s="481"/>
+      <c r="X20" s="481"/>
+      <c r="Y20" s="481"/>
+      <c r="Z20" s="481"/>
+      <c r="AA20" s="481"/>
+      <c r="AB20" s="481"/>
+      <c r="AC20" s="482"/>
       <c r="AZ20" s="311"/>
     </row>
     <row r="21" spans="1:65" ht="12" customHeight="1">
       <c r="A21" s="122"/>
       <c r="B21" s="37"/>
-      <c r="C21" s="491"/>
-      <c r="D21" s="492"/>
-      <c r="E21" s="491"/>
-      <c r="F21" s="498"/>
-      <c r="G21" s="499"/>
-      <c r="H21" s="499"/>
-      <c r="I21" s="499"/>
-      <c r="J21" s="492"/>
+      <c r="C21" s="500"/>
+      <c r="D21" s="576"/>
+      <c r="E21" s="500"/>
+      <c r="F21" s="574"/>
+      <c r="G21" s="575"/>
+      <c r="H21" s="575"/>
+      <c r="I21" s="575"/>
+      <c r="J21" s="576"/>
       <c r="K21" s="69"/>
       <c r="L21" s="102"/>
       <c r="M21" s="103"/>
-      <c r="N21" s="527"/>
-      <c r="O21" s="528"/>
-      <c r="P21" s="491"/>
+      <c r="N21" s="498"/>
+      <c r="O21" s="499"/>
+      <c r="P21" s="500"/>
       <c r="Q21" s="210" t="s">
         <v>151</v>
       </c>
@@ -13207,34 +13207,34 @@
       <c r="T21" s="211" t="s">
         <v>149</v>
       </c>
-      <c r="U21" s="593"/>
-      <c r="V21" s="593"/>
-      <c r="W21" s="593"/>
-      <c r="X21" s="593"/>
-      <c r="Y21" s="593"/>
-      <c r="Z21" s="593"/>
-      <c r="AA21" s="593"/>
-      <c r="AB21" s="593"/>
-      <c r="AC21" s="594"/>
+      <c r="U21" s="514"/>
+      <c r="V21" s="514"/>
+      <c r="W21" s="514"/>
+      <c r="X21" s="514"/>
+      <c r="Y21" s="514"/>
+      <c r="Z21" s="514"/>
+      <c r="AA21" s="514"/>
+      <c r="AB21" s="514"/>
+      <c r="AC21" s="515"/>
       <c r="AZ21" s="311"/>
     </row>
     <row r="22" spans="1:65" ht="12" customHeight="1">
       <c r="A22" s="122"/>
       <c r="B22" s="37"/>
-      <c r="C22" s="491"/>
-      <c r="D22" s="492"/>
-      <c r="E22" s="491"/>
-      <c r="F22" s="498"/>
-      <c r="G22" s="499"/>
-      <c r="H22" s="499"/>
-      <c r="I22" s="499"/>
-      <c r="J22" s="492"/>
+      <c r="C22" s="500"/>
+      <c r="D22" s="576"/>
+      <c r="E22" s="500"/>
+      <c r="F22" s="574"/>
+      <c r="G22" s="575"/>
+      <c r="H22" s="575"/>
+      <c r="I22" s="575"/>
+      <c r="J22" s="576"/>
       <c r="K22" s="69"/>
       <c r="L22" s="102"/>
       <c r="M22" s="103"/>
-      <c r="N22" s="527"/>
-      <c r="O22" s="528"/>
-      <c r="P22" s="491"/>
+      <c r="N22" s="498"/>
+      <c r="O22" s="499"/>
+      <c r="P22" s="500"/>
       <c r="Q22" s="219" t="s">
         <v>150</v>
       </c>
@@ -13243,48 +13243,48 @@
       </c>
       <c r="S22" s="214"/>
       <c r="T22" s="213"/>
-      <c r="U22" s="595"/>
-      <c r="V22" s="595"/>
-      <c r="W22" s="595"/>
-      <c r="X22" s="595"/>
-      <c r="Y22" s="595"/>
-      <c r="Z22" s="595"/>
-      <c r="AA22" s="595"/>
-      <c r="AB22" s="595"/>
-      <c r="AC22" s="596"/>
+      <c r="U22" s="516"/>
+      <c r="V22" s="516"/>
+      <c r="W22" s="516"/>
+      <c r="X22" s="516"/>
+      <c r="Y22" s="516"/>
+      <c r="Z22" s="516"/>
+      <c r="AA22" s="516"/>
+      <c r="AB22" s="516"/>
+      <c r="AC22" s="517"/>
       <c r="AD22" s="86"/>
       <c r="AZ22" s="311"/>
     </row>
     <row r="23" spans="1:65" ht="12" customHeight="1" thickBot="1">
       <c r="A23" s="122"/>
       <c r="B23" s="40"/>
-      <c r="C23" s="491"/>
-      <c r="D23" s="492"/>
-      <c r="E23" s="491"/>
-      <c r="F23" s="498"/>
-      <c r="G23" s="499"/>
-      <c r="H23" s="499"/>
-      <c r="I23" s="499"/>
-      <c r="J23" s="492"/>
+      <c r="C23" s="500"/>
+      <c r="D23" s="576"/>
+      <c r="E23" s="500"/>
+      <c r="F23" s="574"/>
+      <c r="G23" s="575"/>
+      <c r="H23" s="575"/>
+      <c r="I23" s="575"/>
+      <c r="J23" s="576"/>
       <c r="K23" s="70"/>
       <c r="L23" s="70"/>
       <c r="M23" s="104"/>
-      <c r="N23" s="527"/>
-      <c r="O23" s="528"/>
-      <c r="P23" s="491"/>
+      <c r="N23" s="498"/>
+      <c r="O23" s="499"/>
+      <c r="P23" s="500"/>
       <c r="Q23" s="215"/>
       <c r="R23" s="216"/>
       <c r="S23" s="217"/>
       <c r="T23" s="216"/>
-      <c r="U23" s="597"/>
-      <c r="V23" s="597"/>
-      <c r="W23" s="597"/>
-      <c r="X23" s="597"/>
-      <c r="Y23" s="597"/>
-      <c r="Z23" s="597"/>
-      <c r="AA23" s="597"/>
-      <c r="AB23" s="597"/>
-      <c r="AC23" s="598"/>
+      <c r="U23" s="518"/>
+      <c r="V23" s="518"/>
+      <c r="W23" s="518"/>
+      <c r="X23" s="518"/>
+      <c r="Y23" s="518"/>
+      <c r="Z23" s="518"/>
+      <c r="AA23" s="518"/>
+      <c r="AB23" s="518"/>
+      <c r="AC23" s="519"/>
       <c r="AZ23" s="311"/>
     </row>
     <row r="24" spans="1:65" ht="12" customHeight="1" thickBot="1">
@@ -13292,8 +13292,8 @@
         <v>32</v>
       </c>
       <c r="B24" s="56"/>
-      <c r="C24" s="491"/>
-      <c r="D24" s="492"/>
+      <c r="C24" s="500"/>
+      <c r="D24" s="576"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -13305,9 +13305,9 @@
       <c r="K24" s="71"/>
       <c r="L24" s="57"/>
       <c r="M24" s="90"/>
-      <c r="N24" s="524"/>
-      <c r="O24" s="525"/>
-      <c r="P24" s="526"/>
+      <c r="N24" s="577"/>
+      <c r="O24" s="578"/>
+      <c r="P24" s="579"/>
       <c r="Q24" s="175" t="s">
         <v>34</v>
       </c>
@@ -23053,10 +23053,10 @@
       <c r="L99" s="144"/>
       <c r="M99" s="144"/>
       <c r="N99" s="144"/>
-      <c r="O99" s="522" t="s">
+      <c r="O99" s="572" t="s">
         <v>119</v>
       </c>
-      <c r="P99" s="523"/>
+      <c r="P99" s="573"/>
       <c r="Q99" s="148"/>
       <c r="R99" s="148"/>
       <c r="S99" s="148"/>
@@ -23097,10 +23097,10 @@
       <c r="L100" s="144"/>
       <c r="M100" s="144"/>
       <c r="N100" s="144"/>
-      <c r="O100" s="489" t="s">
+      <c r="O100" s="586" t="s">
         <v>118</v>
       </c>
-      <c r="P100" s="490"/>
+      <c r="P100" s="587"/>
       <c r="Q100" s="147"/>
       <c r="R100" s="147"/>
       <c r="S100" s="147"/>
@@ -23197,18 +23197,61 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="S11:U12"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="V9:AA10"/>
+    <mergeCell ref="X11:AA11"/>
+    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="V15:AA16"/>
+    <mergeCell ref="X13:AA13"/>
+    <mergeCell ref="X14:AA14"/>
+    <mergeCell ref="O100:P100"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="C5:G6"/>
+    <mergeCell ref="C7:G8"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="O99:P99"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="S20:AC20"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="W6:X7"/>
+    <mergeCell ref="Y6:Z7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="R5:S7"/>
+    <mergeCell ref="T5:U7"/>
+    <mergeCell ref="M4:P8"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="X17:AC17"/>
     <mergeCell ref="Q18:R19"/>
     <mergeCell ref="N23:P23"/>
     <mergeCell ref="V18:W18"/>
@@ -23225,61 +23268,18 @@
     <mergeCell ref="U21:AC23"/>
     <mergeCell ref="AA18:AC18"/>
     <mergeCell ref="AA19:AC19"/>
-    <mergeCell ref="S20:AC20"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="W6:X7"/>
-    <mergeCell ref="Y6:Z7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="R5:S7"/>
-    <mergeCell ref="T5:U7"/>
-    <mergeCell ref="M4:P8"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="X17:AC17"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="C5:G6"/>
-    <mergeCell ref="C7:G8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="O99:P99"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="O100:P100"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="A13:P13"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="V15:AA16"/>
-    <mergeCell ref="X13:AA13"/>
-    <mergeCell ref="X14:AA14"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="V9:AA10"/>
-    <mergeCell ref="X11:AA11"/>
-    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="Q9:R10"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="S11:U12"/>
   </mergeCells>
   <conditionalFormatting sqref="F27:F97">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
@@ -23696,10 +23696,10 @@
       <c r="A3" s="284" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="537"/>
-      <c r="C3" s="537"/>
-      <c r="D3" s="537"/>
-      <c r="E3" s="537"/>
+      <c r="B3" s="481"/>
+      <c r="C3" s="481"/>
+      <c r="D3" s="481"/>
+      <c r="E3" s="481"/>
       <c r="F3" s="236"/>
       <c r="G3" s="237" t="s">
         <v>47</v>
@@ -28424,10 +28424,10 @@
       <c r="AZ48" s="311"/>
     </row>
     <row r="49" spans="1:52">
-      <c r="A49" s="522" t="s">
+      <c r="A49" s="572" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="523"/>
+      <c r="B49" s="573"/>
       <c r="C49" s="142"/>
       <c r="D49" s="142"/>
       <c r="E49" s="142"/>
@@ -29783,12 +29783,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="636" t="s">
+      <c r="A1" s="654" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="637"/>
-      <c r="C1" s="638"/>
-      <c r="D1" s="639"/>
+      <c r="B1" s="655"/>
+      <c r="C1" s="656"/>
+      <c r="D1" s="657"/>
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
       <c r="G1" s="109"/>
@@ -29858,11 +29858,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="640"/>
-      <c r="D3" s="497"/>
-      <c r="E3" s="497"/>
-      <c r="F3" s="497"/>
-      <c r="G3" s="641"/>
+      <c r="C3" s="658"/>
+      <c r="D3" s="477"/>
+      <c r="E3" s="477"/>
+      <c r="F3" s="477"/>
+      <c r="G3" s="659"/>
       <c r="H3" s="107"/>
       <c r="I3" s="128"/>
       <c r="J3" s="92" t="s">
@@ -29871,10 +29871,10 @@
       <c r="K3" s="108"/>
       <c r="L3" s="108"/>
       <c r="M3" s="108"/>
-      <c r="N3" s="657" t="s">
+      <c r="N3" s="637" t="s">
         <v>117</v>
       </c>
-      <c r="O3" s="658"/>
+      <c r="O3" s="638"/>
       <c r="P3" s="114"/>
       <c r="Q3" s="114"/>
       <c r="R3" s="114"/>
@@ -29895,21 +29895,21 @@
     <row r="4" spans="1:51" ht="12" customHeight="1">
       <c r="A4" s="116"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="560"/>
-      <c r="D4" s="560"/>
-      <c r="E4" s="560"/>
-      <c r="F4" s="560"/>
-      <c r="G4" s="642"/>
-      <c r="H4" s="647" t="s">
+      <c r="C4" s="475"/>
+      <c r="D4" s="475"/>
+      <c r="E4" s="475"/>
+      <c r="F4" s="475"/>
+      <c r="G4" s="660"/>
+      <c r="H4" s="665" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="648"/>
+      <c r="I4" s="666"/>
       <c r="J4" s="108"/>
       <c r="K4" s="108"/>
       <c r="L4" s="108"/>
       <c r="M4" s="108"/>
-      <c r="N4" s="657"/>
-      <c r="O4" s="658"/>
+      <c r="N4" s="637"/>
+      <c r="O4" s="638"/>
       <c r="P4" s="114"/>
       <c r="Q4" s="114"/>
       <c r="R4" s="114"/>
@@ -29932,27 +29932,27 @@
         <v>10</v>
       </c>
       <c r="B5" s="30"/>
-      <c r="C5" s="643"/>
-      <c r="D5" s="559"/>
-      <c r="E5" s="559"/>
-      <c r="F5" s="559"/>
-      <c r="G5" s="644"/>
+      <c r="C5" s="661"/>
+      <c r="D5" s="476"/>
+      <c r="E5" s="476"/>
+      <c r="F5" s="476"/>
+      <c r="G5" s="662"/>
       <c r="H5" s="125" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="645" t="s">
+      <c r="J5" s="663" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="659" t="s">
+      <c r="K5" s="639" t="s">
         <v>100</v>
       </c>
-      <c r="L5" s="659"/>
-      <c r="M5" s="660"/>
-      <c r="N5" s="657"/>
-      <c r="O5" s="658"/>
+      <c r="L5" s="639"/>
+      <c r="M5" s="640"/>
+      <c r="N5" s="637"/>
+      <c r="O5" s="638"/>
       <c r="P5" s="114"/>
       <c r="Q5" s="114"/>
       <c r="R5" s="114"/>
@@ -29973,11 +29973,11 @@
     <row r="6" spans="1:51" ht="12.6" customHeight="1" thickBot="1">
       <c r="A6" s="118"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="560"/>
-      <c r="D6" s="560"/>
-      <c r="E6" s="560"/>
-      <c r="F6" s="560"/>
-      <c r="G6" s="642"/>
+      <c r="C6" s="475"/>
+      <c r="D6" s="475"/>
+      <c r="E6" s="475"/>
+      <c r="F6" s="475"/>
+      <c r="G6" s="660"/>
       <c r="H6" s="126" t="str">
         <f>IF(AND(L11&lt;&gt;0,L10=0),"X","")</f>
         <v/>
@@ -29986,12 +29986,12 @@
         <f>IF(L10=0,"","X")</f>
         <v/>
       </c>
-      <c r="J6" s="646"/>
-      <c r="K6" s="661"/>
-      <c r="L6" s="661"/>
-      <c r="M6" s="662"/>
-      <c r="N6" s="657"/>
-      <c r="O6" s="658"/>
+      <c r="J6" s="664"/>
+      <c r="K6" s="641"/>
+      <c r="L6" s="641"/>
+      <c r="M6" s="642"/>
+      <c r="N6" s="637"/>
+      <c r="O6" s="638"/>
       <c r="P6" s="114"/>
       <c r="Q6" s="114"/>
       <c r="R6" s="114"/>
@@ -30014,19 +30014,19 @@
         <v>14</v>
       </c>
       <c r="B7" s="30"/>
-      <c r="C7" s="643"/>
-      <c r="D7" s="559"/>
-      <c r="E7" s="559"/>
-      <c r="F7" s="559"/>
-      <c r="G7" s="644"/>
+      <c r="C7" s="661"/>
+      <c r="D7" s="476"/>
+      <c r="E7" s="476"/>
+      <c r="F7" s="476"/>
+      <c r="G7" s="662"/>
       <c r="H7" s="305" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="649" t="s">
+      <c r="I7" s="667" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="649"/>
-      <c r="K7" s="650"/>
+      <c r="J7" s="667"/>
+      <c r="K7" s="668"/>
       <c r="L7" s="306">
         <f>COUNTIF($AO$25:$AX$50,"OK")</f>
         <v>0</v>
@@ -30035,8 +30035,8 @@
         <f>IF(($L$7+$L$8)=0,"",L7/($L$7+$L$8))</f>
         <v/>
       </c>
-      <c r="N7" s="657"/>
-      <c r="O7" s="658"/>
+      <c r="N7" s="637"/>
+      <c r="O7" s="638"/>
       <c r="P7" s="114"/>
       <c r="Q7" s="114"/>
       <c r="R7" s="114"/>
@@ -30058,19 +30058,19 @@
     <row r="8" spans="1:51" ht="11.25" customHeight="1">
       <c r="A8" s="119"/>
       <c r="B8" s="38"/>
-      <c r="C8" s="560"/>
-      <c r="D8" s="560"/>
-      <c r="E8" s="560"/>
-      <c r="F8" s="560"/>
-      <c r="G8" s="642"/>
+      <c r="C8" s="475"/>
+      <c r="D8" s="475"/>
+      <c r="E8" s="475"/>
+      <c r="F8" s="475"/>
+      <c r="G8" s="660"/>
       <c r="H8" s="204" t="s">
         <v>209</v>
       </c>
-      <c r="I8" s="649" t="s">
+      <c r="I8" s="667" t="s">
         <v>208</v>
       </c>
-      <c r="J8" s="649"/>
-      <c r="K8" s="650"/>
+      <c r="J8" s="667"/>
+      <c r="K8" s="668"/>
       <c r="L8" s="303">
         <f>COUNTIF($AO$25:$AX$50,"NG")</f>
         <v>0</v>
@@ -30079,8 +30079,8 @@
         <f>IF(($L$7+$L$8)=0,"",L8/($L$7+$L$8))</f>
         <v/>
       </c>
-      <c r="N8" s="657"/>
-      <c r="O8" s="658"/>
+      <c r="N8" s="637"/>
+      <c r="O8" s="638"/>
       <c r="P8" s="114"/>
       <c r="Q8" s="114"/>
       <c r="R8" s="114"/>
@@ -30107,11 +30107,11 @@
       <c r="H9" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="476" t="s">
+      <c r="I9" s="623" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="476"/>
-      <c r="K9" s="477"/>
+      <c r="J9" s="623"/>
+      <c r="K9" s="624"/>
       <c r="L9" s="243">
         <f>COUNTIF($AD$25:$AM$50,"OK")</f>
         <v>0</v>
@@ -30120,8 +30120,8 @@
         <f>IF($L$11=0,"",($L$9/$L$11)*100)</f>
         <v/>
       </c>
-      <c r="N9" s="657"/>
-      <c r="O9" s="658"/>
+      <c r="N9" s="637"/>
+      <c r="O9" s="638"/>
       <c r="P9" s="114"/>
       <c r="Q9" s="114"/>
       <c r="R9" s="114"/>
@@ -30141,24 +30141,24 @@
     </row>
     <row r="10" spans="1:51" ht="12" customHeight="1" thickBot="1">
       <c r="A10" s="121"/>
-      <c r="B10" s="653" t="s">
+      <c r="B10" s="671" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="653"/>
-      <c r="D10" s="608"/>
-      <c r="E10" s="496" t="s">
+      <c r="C10" s="671"/>
+      <c r="D10" s="485"/>
+      <c r="E10" s="591" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="496"/>
-      <c r="G10" s="497"/>
+      <c r="F10" s="591"/>
+      <c r="G10" s="477"/>
       <c r="H10" s="308" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="664" t="s">
+      <c r="I10" s="644" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="664"/>
-      <c r="K10" s="665"/>
+      <c r="J10" s="644"/>
+      <c r="K10" s="645"/>
       <c r="L10" s="309">
         <f>COUNTIF($AD$25:$AM$50,"NG")</f>
         <v>0</v>
@@ -30167,8 +30167,8 @@
         <f>IF($L$11=0,"",($L$10/$L$11)*100)</f>
         <v/>
       </c>
-      <c r="N10" s="657"/>
-      <c r="O10" s="658"/>
+      <c r="N10" s="637"/>
+      <c r="O10" s="638"/>
       <c r="P10" s="114"/>
       <c r="Q10" s="114"/>
       <c r="R10" s="114"/>
@@ -30188,32 +30188,32 @@
     </row>
     <row r="11" spans="1:51" ht="12" customHeight="1">
       <c r="A11" s="121"/>
-      <c r="B11" s="652" t="s">
+      <c r="B11" s="670" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="652"/>
-      <c r="D11" s="639"/>
-      <c r="E11" s="510" t="s">
+      <c r="C11" s="670"/>
+      <c r="D11" s="657"/>
+      <c r="E11" s="600" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="510"/>
-      <c r="G11" s="511"/>
-      <c r="H11" s="666" t="s">
+      <c r="F11" s="600"/>
+      <c r="G11" s="601"/>
+      <c r="H11" s="646" t="s">
         <v>210</v>
       </c>
-      <c r="I11" s="667"/>
-      <c r="J11" s="667"/>
-      <c r="K11" s="668"/>
-      <c r="L11" s="654">
+      <c r="I11" s="647"/>
+      <c r="J11" s="647"/>
+      <c r="K11" s="648"/>
+      <c r="L11" s="652">
         <f>SUM(L9:L10)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="655" t="str">
+      <c r="M11" s="653" t="str">
         <f>IF(L11=0,"",(L11/L11)*100)</f>
         <v/>
       </c>
-      <c r="N11" s="657"/>
-      <c r="O11" s="658"/>
+      <c r="N11" s="637"/>
+      <c r="O11" s="638"/>
       <c r="P11" s="114"/>
       <c r="Q11" s="114"/>
       <c r="R11" s="114"/>
@@ -30239,14 +30239,14 @@
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="669"/>
-      <c r="I12" s="670"/>
-      <c r="J12" s="670"/>
-      <c r="K12" s="671"/>
-      <c r="L12" s="479"/>
-      <c r="M12" s="481"/>
-      <c r="N12" s="657"/>
-      <c r="O12" s="658"/>
+      <c r="H12" s="649"/>
+      <c r="I12" s="650"/>
+      <c r="J12" s="650"/>
+      <c r="K12" s="651"/>
+      <c r="L12" s="603"/>
+      <c r="M12" s="605"/>
+      <c r="N12" s="637"/>
+      <c r="O12" s="638"/>
       <c r="P12" s="114"/>
       <c r="Q12" s="114"/>
       <c r="R12" s="114"/>
@@ -30267,23 +30267,23 @@
       </c>
     </row>
     <row r="13" spans="1:51" ht="12" customHeight="1" thickBot="1">
-      <c r="A13" s="503" t="s">
+      <c r="A13" s="595" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="504"/>
-      <c r="C13" s="504"/>
-      <c r="D13" s="504"/>
-      <c r="E13" s="504"/>
-      <c r="F13" s="504"/>
-      <c r="G13" s="504"/>
-      <c r="H13" s="504"/>
-      <c r="I13" s="504"/>
-      <c r="J13" s="504"/>
-      <c r="K13" s="504"/>
-      <c r="L13" s="504"/>
-      <c r="M13" s="504"/>
-      <c r="N13" s="504"/>
-      <c r="O13" s="651"/>
+      <c r="B13" s="596"/>
+      <c r="C13" s="596"/>
+      <c r="D13" s="596"/>
+      <c r="E13" s="596"/>
+      <c r="F13" s="596"/>
+      <c r="G13" s="596"/>
+      <c r="H13" s="596"/>
+      <c r="I13" s="596"/>
+      <c r="J13" s="596"/>
+      <c r="K13" s="596"/>
+      <c r="L13" s="596"/>
+      <c r="M13" s="596"/>
+      <c r="N13" s="596"/>
+      <c r="O13" s="669"/>
       <c r="P13" s="114"/>
       <c r="Q13" s="114"/>
       <c r="R13" s="114"/>
@@ -30350,19 +30350,19 @@
     <row r="15" spans="1:51" ht="12" customHeight="1">
       <c r="A15" s="122"/>
       <c r="B15" s="39"/>
-      <c r="C15" s="491"/>
-      <c r="D15" s="492"/>
-      <c r="E15" s="491"/>
-      <c r="F15" s="498"/>
-      <c r="G15" s="499"/>
-      <c r="H15" s="499"/>
-      <c r="I15" s="499"/>
-      <c r="J15" s="492"/>
+      <c r="C15" s="500"/>
+      <c r="D15" s="576"/>
+      <c r="E15" s="500"/>
+      <c r="F15" s="574"/>
+      <c r="G15" s="575"/>
+      <c r="H15" s="575"/>
+      <c r="I15" s="575"/>
+      <c r="J15" s="576"/>
       <c r="K15" s="69"/>
       <c r="L15" s="102"/>
       <c r="M15" s="102"/>
-      <c r="N15" s="528"/>
-      <c r="O15" s="529"/>
+      <c r="N15" s="499"/>
+      <c r="O15" s="513"/>
       <c r="P15" s="114"/>
       <c r="Q15" s="114"/>
       <c r="R15" s="114"/>
@@ -30380,19 +30380,19 @@
     <row r="16" spans="1:51" ht="12" customHeight="1">
       <c r="A16" s="122"/>
       <c r="B16" s="39"/>
-      <c r="C16" s="491"/>
-      <c r="D16" s="492"/>
-      <c r="E16" s="491"/>
-      <c r="F16" s="498"/>
-      <c r="G16" s="499"/>
-      <c r="H16" s="499"/>
-      <c r="I16" s="499"/>
-      <c r="J16" s="492"/>
+      <c r="C16" s="500"/>
+      <c r="D16" s="576"/>
+      <c r="E16" s="500"/>
+      <c r="F16" s="574"/>
+      <c r="G16" s="575"/>
+      <c r="H16" s="575"/>
+      <c r="I16" s="575"/>
+      <c r="J16" s="576"/>
       <c r="K16" s="69"/>
       <c r="L16" s="102"/>
       <c r="M16" s="102"/>
-      <c r="N16" s="528"/>
-      <c r="O16" s="529"/>
+      <c r="N16" s="499"/>
+      <c r="O16" s="513"/>
       <c r="P16" s="114"/>
       <c r="Q16" s="114"/>
       <c r="R16" s="114"/>
@@ -30421,8 +30421,8 @@
       <c r="K17" s="69"/>
       <c r="L17" s="102"/>
       <c r="M17" s="102"/>
-      <c r="N17" s="528"/>
-      <c r="O17" s="529"/>
+      <c r="N17" s="499"/>
+      <c r="O17" s="513"/>
       <c r="P17" s="114"/>
       <c r="Q17" s="114"/>
       <c r="R17" s="114"/>
@@ -30451,8 +30451,8 @@
       <c r="K18" s="69"/>
       <c r="L18" s="102"/>
       <c r="M18" s="102"/>
-      <c r="N18" s="528"/>
-      <c r="O18" s="529"/>
+      <c r="N18" s="499"/>
+      <c r="O18" s="513"/>
       <c r="P18" s="114"/>
       <c r="Q18" s="114"/>
       <c r="R18" s="114"/>
@@ -30481,8 +30481,8 @@
       <c r="K19" s="69"/>
       <c r="L19" s="102"/>
       <c r="M19" s="102"/>
-      <c r="N19" s="528"/>
-      <c r="O19" s="529"/>
+      <c r="N19" s="499"/>
+      <c r="O19" s="513"/>
       <c r="P19" s="114"/>
       <c r="Q19" s="114"/>
       <c r="R19" s="114"/>
@@ -30511,8 +30511,8 @@
       <c r="K20" s="69"/>
       <c r="L20" s="102"/>
       <c r="M20" s="102"/>
-      <c r="N20" s="528"/>
-      <c r="O20" s="529"/>
+      <c r="N20" s="499"/>
+      <c r="O20" s="513"/>
       <c r="P20" s="114"/>
       <c r="Q20" s="114"/>
       <c r="R20" s="114"/>
@@ -30530,19 +30530,19 @@
     <row r="21" spans="1:52" ht="12" customHeight="1" thickBot="1">
       <c r="A21" s="122"/>
       <c r="B21" s="37"/>
-      <c r="C21" s="491"/>
-      <c r="D21" s="492"/>
-      <c r="E21" s="491"/>
-      <c r="F21" s="498"/>
-      <c r="G21" s="499"/>
-      <c r="H21" s="499"/>
-      <c r="I21" s="499"/>
-      <c r="J21" s="492"/>
+      <c r="C21" s="500"/>
+      <c r="D21" s="576"/>
+      <c r="E21" s="500"/>
+      <c r="F21" s="574"/>
+      <c r="G21" s="575"/>
+      <c r="H21" s="575"/>
+      <c r="I21" s="575"/>
+      <c r="J21" s="576"/>
       <c r="K21" s="69"/>
       <c r="L21" s="102"/>
       <c r="M21" s="102"/>
-      <c r="N21" s="528"/>
-      <c r="O21" s="529"/>
+      <c r="N21" s="499"/>
+      <c r="O21" s="513"/>
       <c r="P21" s="115"/>
       <c r="Q21" s="115"/>
       <c r="R21" s="115"/>
@@ -30562,8 +30562,8 @@
         <v>32</v>
       </c>
       <c r="B22" s="56"/>
-      <c r="C22" s="526"/>
-      <c r="D22" s="656"/>
+      <c r="C22" s="579"/>
+      <c r="D22" s="636"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -30575,8 +30575,8 @@
       <c r="K22" s="71"/>
       <c r="L22" s="57"/>
       <c r="M22" s="101"/>
-      <c r="N22" s="525"/>
-      <c r="O22" s="663"/>
+      <c r="N22" s="578"/>
+      <c r="O22" s="643"/>
       <c r="P22" s="14" t="s">
         <v>34</v>
       </c>
@@ -33946,10 +33946,10 @@
       <c r="L52" s="144"/>
       <c r="M52" s="144"/>
       <c r="N52" s="144"/>
-      <c r="O52" s="522" t="s">
+      <c r="O52" s="572" t="s">
         <v>119</v>
       </c>
-      <c r="P52" s="523"/>
+      <c r="P52" s="573"/>
       <c r="Q52" s="148"/>
       <c r="R52" s="148"/>
       <c r="S52" s="148"/>
@@ -34109,6 +34109,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="C5:G6"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C7:G8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
     <mergeCell ref="O53:P53"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="N15:O15"/>
@@ -34125,28 +34147,6 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="H11:K12"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="C5:G6"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="C7:G8"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="F25:F50">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
@@ -34295,6 +34295,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B39C76C5F415C48BD1EE1EAF5952407" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4bec31a393816f4b6c8fd25bd674081">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -34408,32 +34423,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F83C9-2640-4592-845A-16A932EECE94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8BC4E0A-9566-4C3C-AE1F-FA992E0C888C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -34448,9 +34441,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8BC4E0A-9566-4C3C-AE1F-FA992E0C888C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3F83C9-2640-4592-845A-16A932EECE94}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>